<commit_message>
Se actualiza A2_Compiler.py para utilizar pandas 2.0.3 bajo conda 23.7.4.
</commit_message>
<xml_diff>
--- a/Energia/Model/t1_confection/A2_Structure_Lists.xlsx
+++ b/Energia/Model/t1_confection/A2_Structure_Lists.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="403">
   <si>
     <t>Year</t>
   </si>
@@ -1207,25 +1207,19 @@
     <t>DEMTRN_NOMOT</t>
   </si>
   <si>
+    <t>Congestion</t>
+  </si>
+  <si>
+    <t>Accidents</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
     <t>CO2_fugitivas</t>
-  </si>
-  <si>
-    <t>Health</t>
-  </si>
-  <si>
-    <t>Accidents</t>
-  </si>
-  <si>
-    <t>Congestion</t>
-  </si>
-  <si>
-    <t>CO2_scc</t>
-  </si>
-  <si>
-    <t>CO2_fugitivas_scc</t>
-  </si>
-  <si>
-    <t>CO2</t>
   </si>
   <si>
     <t>ECU</t>
@@ -1635,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1704,9 +1698,6 @@
       <c r="D7" t="s">
         <v>272</v>
       </c>
-      <c r="E7" t="s">
-        <v>402</v>
-      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
@@ -1717,9 +1708,6 @@
       </c>
       <c r="D8" t="s">
         <v>273</v>
-      </c>
-      <c r="E8" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:7">

</xml_diff>